<commit_message>
Se agrega el Plan de Calidad y Matriz de Riesgos Actualizado
</commit_message>
<xml_diff>
--- a/Plan de Calidad Reto.xlsx
+++ b/Plan de Calidad Reto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA919570-93E2-4476-B07E-F65B8DF40C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CB1E17-3138-425B-8B85-7E79649291C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="155">
   <si>
     <t xml:space="preserve">Area </t>
   </si>
@@ -109,9 +109,6 @@
     <t>Plan de Acción</t>
   </si>
   <si>
-    <t>Responsable de la Acción</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fecha Compromiso </t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Durante el Sprint</t>
   </si>
   <si>
-    <t>Abierto</t>
-  </si>
-  <si>
     <t>Producto</t>
   </si>
   <si>
@@ -274,13 +268,7 @@
     <t>Equipo de Pruebas Sofka</t>
   </si>
   <si>
-    <t>Registro de clientes expuesto a vulnerabilidades de seguridad</t>
-  </si>
-  <si>
     <t>Alta demanda de usuarios que intenten hacer registro simultáneamente</t>
-  </si>
-  <si>
-    <t>Interfaz de registro poco intuitiva o difícil de usar para los usuarios</t>
   </si>
   <si>
     <t>Intento de registro de información  falsa o robada</t>
@@ -362,9 +350,6 @@
 Redefinir o ajustar el proyecto de acuerdo a la normatividad.</t>
   </si>
   <si>
-    <t>PO/Amazon</t>
-  </si>
-  <si>
     <t>Durante todo el proyecto</t>
   </si>
   <si>
@@ -407,13 +392,7 @@
     <t xml:space="preserve">Realizar pruebas de carga y rendimiento en el sitio web para identificar cuellos de botella, tiempos de carga y rendimiento general del sitio. </t>
   </si>
   <si>
-    <t>Equipo QA</t>
-  </si>
-  <si>
     <t>Añadir alertas de inventario bajo para que los administradores puedan recibir notificaciones cuando un producto está cerca de quedarse sin stock.</t>
-  </si>
-  <si>
-    <t>Equipo Desarrollo</t>
   </si>
   <si>
     <t>Realizar pruebas rigurosas de rendimiento antes del lanzamiento para garantizar que pueda manejar el tráfico de usuarios</t>
@@ -463,10 +442,6 @@
   </si>
   <si>
     <t>Implementar herramientas de diseño responsive para adaptar automáticamente el sitio web a diferentes tamaños de pantalla.</t>
-  </si>
-  <si>
-    <t>Equipo Desarrollo
-Equipo QA</t>
   </si>
   <si>
     <t>Retrasos en la adquisición o configuración de herramientas y recursos necesarios para el proyecto</t>
@@ -525,6 +500,33 @@
 *Verificar que no permita ingresar una tarjeta invalida como metodo de pago.
 *Verificar que no permita ingresar una direccion de envio invalida.
 *Verificar que no permita agregar una cantidad de stock mayor al disponible de un producto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La integración con sistemas externos que no estén contemplados en el alcance.
+La validación de aspectos legales, como términos y condiciones, políticas de privacidad, entre otros, que no estén especificados en el alcance.
+Las pruebas de dispositivos móviles que no estén especificados en el alcance.
+Todo aquello que no este definido dentro del alcance.
+No se probará en otros navegadores que no sean Chrome
+Los factores no funcionales como el rendimiento, la seguridad informática, la usabilidad, la escalabilidad.
+</t>
+  </si>
+  <si>
+    <t>Para el servicio SOAP de calculadora se implementara la siguiente estrategia.
+Laspruebas se realizaran manualmente.
+1. Identificar los escenarios más comunes para cada operación de la calculadora (sumar, restar, multiplicar y dividir).
+2. Crear escenarios para probar cada una de estas operaciones con diferentes tipos de datos (números positivos y negativos, decimales, cero, etc.).
+3. Verificar la capacidad del servicio para manejar casos de error, como entradas incorrectas o divisiones por cero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Acceso al ambiente de produccion de Amazon.com.
+2. Casos de prueba predefinidos
+</t>
+  </si>
+  <si>
+    <t>Se parte del supuesto que todas las funcionalidades que involucran el flujo de compra de un producto en amazon esten funcionando.</t>
+  </si>
+  <si>
+    <t>Juan David Cardona</t>
   </si>
   <si>
     <r>
@@ -549,6 +551,7 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">*Verificar que se sumen de manera correcta 2 numeros positivos.
+*Verficiar que se sumen de manera correcta 2 numeros decimales.
 *Verificar que se sumen de manera correcta 1 numero positivo y 1 numero negativos.
 *Verificar que se sumen de manera correcta 2 numeros negativos.
 *Verificar que se resten de manera correcta 2 numeros positivos.
@@ -566,45 +569,24 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">La integración con sistemas externos que no estén contemplados en el alcance.
-La validación de aspectos legales, como términos y condiciones, políticas de privacidad, entre otros, que no estén especificados en el alcance.
-Las pruebas de dispositivos móviles que no estén especificados en el alcance.
-Todo aquello que no este definido dentro del alcance.
-No se probará en otros navegadores que no sean Chrome
-Los factores no funcionales como el rendimiento, la seguridad informática, la usabilidad, la escalabilidad.
-</t>
-  </si>
-  <si>
-    <t>Para el servicio SOAP de calculadora se implementara la siguiente estrategia.
-Laspruebas se realizaran manualmente.
-1. Identificar los escenarios más comunes para cada operación de la calculadora (sumar, restar, multiplicar y dividir).
-2. Crear escenarios para probar cada una de estas operaciones con diferentes tipos de datos (números positivos y negativos, decimales, cero, etc.).
-3. Verificar la capacidad del servicio para manejar casos de error, como entradas incorrectas o divisiones por cero.</t>
-  </si>
-  <si>
-    <t>Identificación de los requisitos de prueba: se debe identificar los requisitos del flujo de compra para definir el alcance de las pruebas y la documentación de las pruebas.
-Diseño de casos de prueba: se deben diseñar casos de prueba para cada uno de los requisitos mencionados. Cada caso de prueba debe estar diseñado para verificar un requisito específico del flujo de compra.
-Preparación del ambiente de prueba: se debe preparar el ambiente de prueba con los datos y las configuraciones necesarias para la ejecución de los casos de prueba.
-Ejecución de pruebas: se deben ejecutar los casos de prueba diseñados en el paso anterior y se deben documentar los resultados de cada prueba.
-Análisis de los resultados de prueba: se deben analizar los resultados de las pruebas y se deben identificar los defectos encontrados durante la ejecución de los casos de prueba.
-Validación del resultado de prueba: se deben validar que todos los requisitos del flujo de compra se hayan cumplido y que no se hayan generado nuevos problemas después de la corrección de defectos y retesting.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Acceso al ambiente de produccion de Amazon.com.
-2. Casos de prueba predefinidos
-</t>
-  </si>
-  <si>
-    <t>Se parte del supuesto que todas las funcionalidades que involucran el flujo de compra de un producto en amazon esten funcionando.</t>
+    <t>1.Identificación de los requisitos de prueba: se debe identificar los requisitos del flujo de compra para definir el alcance de las pruebas y la documentación de las pruebas.
+2. Diseño de casos de prueba: se deben diseñar casos de prueba para cada uno de los requisitos mencionados. Cada caso de prueba debe estar diseñado para verificar un requisito específico del flujo de compra.
+3.Preparación del ambiente de prueba: se debe preparar el ambiente de prueba con los datos y las configuraciones necesarias para la ejecución de los casos de prueba.
+4.Ejecución de pruebas: se deben ejecutar los casos de prueba diseñados en el paso anterior y se deben documentar los resultados de cada prueba.
+5.Análisis de los resultados de prueba: se deben analizar los resultados de las pruebas y se deben identificar los defectos encontrados durante la ejecución de los casos de prueba.
+Las pruebas se haran de forma manual.</t>
+  </si>
+  <si>
+    <t>Inicio de sesion de clientes expuesto a vulnerabilidades de seguridad</t>
+  </si>
+  <si>
+    <t>Interfaz de login poco intuitiva o difícil de usar para los usuarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-  </numFmts>
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -755,7 +737,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -861,11 +843,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -932,30 +955,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -967,9 +966,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1004,99 +1000,34 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="61">
     <dxf>
       <font>
         <color rgb="FF92D050"/>
@@ -1129,48 +1060,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1353,6 +1242,60 @@
         <charset val="134"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1381,6 +1324,48 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1670,59 +1655,59 @@
   </dxfs>
   <tableStyles count="11">
     <tableStyle name="Matriz de Riesgo -style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="62"/>
-      <tableStyleElement type="firstRowStripe" dxfId="61"/>
-      <tableStyleElement type="secondRowStripe" dxfId="60"/>
+      <tableStyleElement type="headerRow" dxfId="60"/>
+      <tableStyleElement type="firstRowStripe" dxfId="59"/>
+      <tableStyleElement type="secondRowStripe" dxfId="58"/>
     </tableStyle>
     <tableStyle name="Ejemplo Matriz de Riesgo-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="59"/>
-      <tableStyleElement type="firstRowStripe" dxfId="58"/>
-      <tableStyleElement type="secondRowStripe" dxfId="57"/>
+      <tableStyleElement type="headerRow" dxfId="57"/>
+      <tableStyleElement type="firstRowStripe" dxfId="56"/>
+      <tableStyleElement type="secondRowStripe" dxfId="55"/>
     </tableStyle>
     <tableStyle name="Instructivo-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="56"/>
-      <tableStyleElement type="firstRowStripe" dxfId="55"/>
-      <tableStyleElement type="secondRowStripe" dxfId="54"/>
+      <tableStyleElement type="headerRow" dxfId="54"/>
+      <tableStyleElement type="firstRowStripe" dxfId="53"/>
+      <tableStyleElement type="secondRowStripe" dxfId="52"/>
     </tableStyle>
     <tableStyle name="Tabla-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="53"/>
-      <tableStyleElement type="firstRowStripe" dxfId="52"/>
-      <tableStyleElement type="secondRowStripe" dxfId="51"/>
+      <tableStyleElement type="headerRow" dxfId="51"/>
+      <tableStyleElement type="firstRowStripe" dxfId="50"/>
+      <tableStyleElement type="secondRowStripe" dxfId="49"/>
     </tableStyle>
     <tableStyle name="Tabla-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="50"/>
-      <tableStyleElement type="firstRowStripe" dxfId="49"/>
-      <tableStyleElement type="secondRowStripe" dxfId="48"/>
+      <tableStyleElement type="headerRow" dxfId="48"/>
+      <tableStyleElement type="firstRowStripe" dxfId="47"/>
+      <tableStyleElement type="secondRowStripe" dxfId="46"/>
     </tableStyle>
     <tableStyle name="Tabla-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="47"/>
-      <tableStyleElement type="firstRowStripe" dxfId="46"/>
-      <tableStyleElement type="secondRowStripe" dxfId="45"/>
+      <tableStyleElement type="headerRow" dxfId="45"/>
+      <tableStyleElement type="firstRowStripe" dxfId="44"/>
+      <tableStyleElement type="secondRowStripe" dxfId="43"/>
     </tableStyle>
     <tableStyle name="Tabla-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="44"/>
-      <tableStyleElement type="firstRowStripe" dxfId="43"/>
-      <tableStyleElement type="secondRowStripe" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="42"/>
+      <tableStyleElement type="firstRowStripe" dxfId="41"/>
+      <tableStyleElement type="secondRowStripe" dxfId="40"/>
     </tableStyle>
     <tableStyle name="Tabla-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
-      <tableStyleElement type="headerRow" dxfId="41"/>
-      <tableStyleElement type="firstRowStripe" dxfId="40"/>
-      <tableStyleElement type="secondRowStripe" dxfId="39"/>
+      <tableStyleElement type="headerRow" dxfId="39"/>
+      <tableStyleElement type="firstRowStripe" dxfId="38"/>
+      <tableStyleElement type="secondRowStripe" dxfId="37"/>
     </tableStyle>
     <tableStyle name="Tabla-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
-      <tableStyleElement type="headerRow" dxfId="38"/>
-      <tableStyleElement type="firstRowStripe" dxfId="37"/>
-      <tableStyleElement type="secondRowStripe" dxfId="36"/>
+      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="firstRowStripe" dxfId="35"/>
+      <tableStyleElement type="secondRowStripe" dxfId="34"/>
     </tableStyle>
     <tableStyle name="Tabla-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="firstRowStripe" dxfId="34"/>
-      <tableStyleElement type="secondRowStripe" dxfId="33"/>
+      <tableStyleElement type="headerRow" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
     <tableStyle name="Tabla-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0A000000}">
-      <tableStyleElement type="headerRow" dxfId="32"/>
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
-      <tableStyleElement type="secondRowStripe" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="30"/>
+      <tableStyleElement type="firstRowStripe" dxfId="29"/>
+      <tableStyleElement type="secondRowStripe" dxfId="28"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1973,7 +1958,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="16715740" cy="895350"/>
+    <xdr:ext cx="14591665" cy="895350"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="Shape 4">
@@ -1988,7 +1973,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="635" y="171450"/>
-          <a:ext cx="16715740" cy="895350"/>
+          <a:ext cx="14591665" cy="895350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2029,13 +2014,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>771525</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2076,15 +2061,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1009650</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2107,7 +2092,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7677150" y="27670125"/>
+          <a:off x="8115300" y="27393900"/>
           <a:ext cx="3057525" cy="2057400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2169,25 +2154,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_2" displayName="Table_2" ref="A7:M39" headerRowDxfId="29">
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Consecutivo" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción Riesgo" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tipo de Riesgo" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Release" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Probabilidad de ocurrencia" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Impacto" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Riesgo" dataDxfId="25">
-      <calculatedColumnFormula>'Matriz de Riesgo'!$E$8:$E$39*'Matriz de Riesgo'!$F$8:$F$39</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_2" displayName="Table_2" ref="A7:K37" headerRowDxfId="27">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Consecutivo" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción Riesgo" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tipo de Riesgo" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Release" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Probabilidad de ocurrencia" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Impacto" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Riesgo" dataDxfId="20">
+      <calculatedColumnFormula>'Matriz de Riesgo'!$E$8:$E$37*'Matriz de Riesgo'!$F$8:$F$37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Riesgo " dataDxfId="5">
-      <calculatedColumnFormula>'Matriz de Riesgo'!$G$8:$G$39</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Riesgo " dataDxfId="19">
+      <calculatedColumnFormula>'Matriz de Riesgo'!$G$8:$G$37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Acción" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Plan de Acción" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Responsable de la Acción" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Fecha Compromiso " dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Estado" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Acción" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Plan de Acción" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Fecha Compromiso " dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Ejemplo Matriz de Riesgo-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2196,8 +2179,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_4" displayName="Table_4" ref="A1:B5">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Plan de Acción" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Descripción" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Plan de Acción" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Descripción" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2206,7 +2189,7 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_5" displayName="Table_5" ref="D1:D3">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Tipo de Riesg" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Tipo de Riesg" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2215,9 +2198,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_6" displayName="Table_6" ref="F1:H6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Probabilidad" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Evaluación" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Definición" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Probabilidad" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Evaluación" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Definición" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2226,9 +2209,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_7" displayName="Table_7" ref="J1:L6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Impacto" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Evaluación" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Definición" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Impacto" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Evaluación" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Definición" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2237,7 +2220,7 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_8" displayName="Table_8" ref="A8:A10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Responsable Calidad" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Responsable Calidad" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2246,7 +2229,7 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_9" displayName="Table_9" ref="D8:D10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Plan de Calidad" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Plan de Calidad" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2255,7 +2238,7 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table_10" displayName="Table_10" ref="F8:F10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Historia de Usuario" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Historia de Usuario" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2264,7 +2247,7 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_11" displayName="Table_11" ref="A12:A14">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Estado" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Estado" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2474,14 +2457,14 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25.140625" style="9" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="9" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="9" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="9" customWidth="1"/>
     <col min="6" max="6" width="41.140625" style="9" customWidth="1"/>
@@ -2495,34 +2478,34 @@
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:13" ht="14.25" customHeight="1">
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" customHeight="1">
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="1:13" ht="14.25" customHeight="1">
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
     </row>
     <row r="5" spans="1:13" ht="14.25" customHeight="1">
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
     </row>
     <row r="6" spans="1:13" ht="14.25" customHeight="1">
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
     </row>
     <row r="7" spans="1:13" s="8" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
@@ -2567,84 +2550,84 @@
     </row>
     <row r="8" spans="1:13" ht="369" customHeight="1" thickBot="1">
       <c r="A8" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="11" t="s">
         <v>75</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>73</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H8" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="M8" s="15" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="409.5" customHeight="1">
       <c r="A9" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>13</v>
+        <v>76</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="172.5" customHeight="1">
@@ -3666,13 +3649,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>Tabla!$A$9:$A$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>C9</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Tabla!$D$9:$D$10</xm:f>
@@ -3690,16 +3667,16 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:M1000"/>
+  <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" style="43" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" style="32" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="7.140625" style="8" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" style="26" customWidth="1"/>
@@ -3708,103 +3685,89 @@
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="8" customWidth="1"/>
     <col min="10" max="10" width="37.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="8" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="8" customWidth="1"/>
-    <col min="14" max="26" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="8" customWidth="1"/>
+    <col min="12" max="24" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A1" s="31"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
+    <row r="1" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
     </row>
-    <row r="2" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
+    <row r="2" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
     </row>
-    <row r="3" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+    <row r="3" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
     </row>
-    <row r="4" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
+    <row r="4" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
     </row>
-    <row r="5" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
+    <row r="5" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A5" s="45"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
     </row>
-    <row r="6" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
+    <row r="6" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A6" s="45"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
     </row>
-    <row r="7" spans="1:13" ht="27" customHeight="1">
+    <row r="7" spans="1:11" ht="27" customHeight="1">
       <c r="A7" s="22" t="s">
         <v>15</v>
       </c>
@@ -3838,22 +3801,16 @@
       <c r="K7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="8" spans="1:13" ht="75" customHeight="1">
+    <row r="8" spans="1:11" ht="75" customHeight="1">
       <c r="A8" s="8">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>112</v>
+      <c r="B8" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
@@ -3873,30 +3830,24 @@
         <v>15</v>
       </c>
       <c r="I8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="54" t="s">
-        <v>151</v>
-      </c>
-      <c r="K8" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="9" spans="1:13" ht="44.25" customHeight="1">
+    <row r="9" spans="1:11" ht="53.25" customHeight="1">
       <c r="A9" s="8">
         <v>2</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>79</v>
+      <c r="B9" s="51" t="s">
+        <v>153</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
@@ -3916,30 +3867,24 @@
         <v>12</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="M9" s="55" t="s">
-        <v>30</v>
+        <v>80</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="44.25" customHeight="1">
+    <row r="10" spans="1:11" ht="44.25" customHeight="1">
       <c r="A10" s="24">
         <v>3</v>
       </c>
-      <c r="B10" s="38" t="s">
-        <v>80</v>
+      <c r="B10" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="24">
         <v>1</v>
@@ -3959,30 +3904,24 @@
         <v>20</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="K10" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="M10" s="24" t="s">
-        <v>30</v>
+        <v>116</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75.75" customHeight="1">
+    <row r="11" spans="1:11" ht="75.75" customHeight="1">
       <c r="A11" s="24">
         <v>4</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="24">
         <v>1</v>
@@ -4002,30 +3941,24 @@
         <v>16</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" s="24" t="s">
-        <v>30</v>
+        <v>91</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="44.25" customHeight="1">
+    <row r="12" spans="1:11" ht="44.25" customHeight="1">
       <c r="A12" s="24">
         <v>5</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>81</v>
+      <c r="B12" s="31" t="s">
+        <v>154</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="24">
         <v>1</v>
@@ -4045,30 +3978,24 @@
         <v>6</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="K12" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="M12" s="24" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60.75" customHeight="1">
+    <row r="13" spans="1:11" ht="60.75" customHeight="1">
       <c r="A13" s="24">
         <v>6</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>82</v>
+      <c r="B13" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="24">
         <v>1</v>
@@ -4088,30 +4015,24 @@
         <v>20</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>30</v>
+        <v>82</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="46.5" customHeight="1">
+    <row r="14" spans="1:11" ht="46.5" customHeight="1">
       <c r="A14" s="24">
         <v>7</v>
       </c>
-      <c r="B14" s="44" t="s">
-        <v>87</v>
+      <c r="B14" s="33" t="s">
+        <v>83</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="24">
         <v>1</v>
@@ -4131,30 +4052,24 @@
         <v>10</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="L14" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="47.25" customHeight="1">
+    <row r="15" spans="1:11" ht="47.25" customHeight="1">
       <c r="A15" s="24">
         <v>8</v>
       </c>
-      <c r="B15" s="44" t="s">
-        <v>89</v>
+      <c r="B15" s="33" t="s">
+        <v>85</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="24">
         <v>1</v>
@@ -4174,30 +4089,24 @@
         <v>12</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="55.5" customHeight="1">
+    <row r="16" spans="1:11" ht="55.5" customHeight="1">
       <c r="A16" s="24">
         <v>9</v>
       </c>
-      <c r="B16" s="39" t="s">
-        <v>91</v>
+      <c r="B16" s="29" t="s">
+        <v>87</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="24">
         <v>1</v>
@@ -4217,30 +4126,24 @@
         <v>8</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="M16" s="24" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="30" customHeight="1">
+    <row r="17" spans="1:11" ht="30" customHeight="1">
       <c r="A17" s="24">
         <v>10</v>
       </c>
-      <c r="B17" s="40" t="s">
-        <v>93</v>
+      <c r="B17" s="30" t="s">
+        <v>89</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="24">
         <v>1</v>
@@ -4260,38 +4163,32 @@
         <v>10</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="L17" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="M17" s="24" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="57.75" customHeight="1">
+    <row r="18" spans="1:11" ht="57.75" customHeight="1">
       <c r="A18" s="24">
         <v>11</v>
       </c>
-      <c r="B18" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="46">
+      <c r="B18" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="35">
         <v>1</v>
       </c>
-      <c r="E18" s="46">
+      <c r="E18" s="35">
         <v>3</v>
       </c>
-      <c r="F18" s="46">
+      <c r="F18" s="35">
         <v>4</v>
       </c>
       <c r="G18" s="25">
@@ -4302,39 +4199,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$19</f>
         <v>12</v>
       </c>
-      <c r="I18" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J18" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="K18" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L18" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M18" s="24" t="s">
-        <v>30</v>
+      <c r="I18" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="K18" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="64.5" customHeight="1">
+    <row r="19" spans="1:11" ht="64.5" customHeight="1">
       <c r="A19" s="24">
         <v>12</v>
       </c>
-      <c r="B19" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="46">
+      <c r="B19" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="35">
         <v>1</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="35">
         <v>3</v>
       </c>
-      <c r="F19" s="46">
+      <c r="F19" s="35">
         <v>3</v>
       </c>
       <c r="G19" s="25">
@@ -4345,39 +4236,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$19</f>
         <v>9</v>
       </c>
-      <c r="I19" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="K19" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="L19" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M19" s="24" t="s">
-        <v>30</v>
+      <c r="I19" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="K19" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="66.75" customHeight="1">
+    <row r="20" spans="1:11" ht="66.75" customHeight="1">
       <c r="A20" s="24">
         <v>13</v>
       </c>
-      <c r="B20" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="46">
+      <c r="B20" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="35">
         <v>1</v>
       </c>
-      <c r="E20" s="46">
+      <c r="E20" s="35">
         <v>4</v>
       </c>
-      <c r="F20" s="46">
+      <c r="F20" s="35">
         <v>2</v>
       </c>
       <c r="G20" s="25">
@@ -4388,39 +4273,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>8</v>
       </c>
-      <c r="I20" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="K20" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="L20" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M20" s="24" t="s">
-        <v>30</v>
+      <c r="I20" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="67.5" customHeight="1">
+    <row r="21" spans="1:11" ht="67.5" customHeight="1">
       <c r="A21" s="24">
         <v>14</v>
       </c>
-      <c r="B21" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="46">
+      <c r="B21" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="35">
         <v>1</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="35">
         <v>2</v>
       </c>
-      <c r="F21" s="46">
+      <c r="F21" s="35">
         <v>3</v>
       </c>
       <c r="G21" s="25">
@@ -4431,39 +4310,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$26</f>
         <v>6</v>
       </c>
-      <c r="I21" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="K21" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="L21" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M21" s="24" t="s">
-        <v>30</v>
+      <c r="I21" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="K21" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="64.5" customHeight="1">
+    <row r="22" spans="1:11" ht="64.5" customHeight="1">
       <c r="A22" s="24">
         <v>15</v>
       </c>
-      <c r="B22" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="46">
+      <c r="B22" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="35">
         <v>1</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="35">
         <v>3</v>
       </c>
-      <c r="F22" s="46">
+      <c r="F22" s="35">
         <v>4</v>
       </c>
       <c r="G22" s="25">
@@ -4474,37 +4347,31 @@
         <f>'Matriz de Riesgo'!$G$8:$G$26</f>
         <v>12</v>
       </c>
-      <c r="I22" s="46"/>
-      <c r="J22" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="K22" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="L22" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M22" s="24" t="s">
-        <v>30</v>
+      <c r="I22" s="35"/>
+      <c r="J22" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="58.5" customHeight="1">
+    <row r="23" spans="1:11" ht="58.5" customHeight="1">
       <c r="A23" s="24">
         <v>16</v>
       </c>
-      <c r="B23" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="46">
+      <c r="B23" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="35">
         <v>1</v>
       </c>
-      <c r="E23" s="46">
+      <c r="E23" s="35">
         <v>4</v>
       </c>
-      <c r="F23" s="46">
+      <c r="F23" s="35">
         <v>5</v>
       </c>
       <c r="G23" s="25">
@@ -4515,37 +4382,31 @@
         <f>'Matriz de Riesgo'!$G$8:$G$26</f>
         <v>20</v>
       </c>
-      <c r="I23" s="46"/>
-      <c r="J23" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="K23" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L23" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M23" s="24" t="s">
-        <v>30</v>
+      <c r="I23" s="35"/>
+      <c r="J23" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="K23" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="105" customHeight="1">
+    <row r="24" spans="1:11" ht="105" customHeight="1">
       <c r="A24" s="24">
         <v>17</v>
       </c>
-      <c r="B24" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="46">
+      <c r="B24" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="35">
         <v>1</v>
       </c>
-      <c r="E24" s="46">
+      <c r="E24" s="35">
         <v>3</v>
       </c>
-      <c r="F24" s="46">
+      <c r="F24" s="35">
         <v>3</v>
       </c>
       <c r="G24" s="25">
@@ -4556,39 +4417,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$26</f>
         <v>9</v>
       </c>
-      <c r="I24" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J24" s="47" t="s">
-        <v>128</v>
-      </c>
-      <c r="K24" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L24" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M24" s="24" t="s">
-        <v>30</v>
+      <c r="I24" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="102" customHeight="1">
+    <row r="25" spans="1:11" ht="102" customHeight="1">
       <c r="A25" s="24">
         <v>18</v>
       </c>
-      <c r="B25" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="C25" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="46">
+      <c r="B25" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="35">
         <v>1</v>
       </c>
-      <c r="E25" s="46">
+      <c r="E25" s="35">
         <v>4</v>
       </c>
-      <c r="F25" s="46">
+      <c r="F25" s="35">
         <v>5</v>
       </c>
       <c r="G25" s="25">
@@ -4599,39 +4454,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$26</f>
         <v>20</v>
       </c>
-      <c r="I25" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J25" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="K25" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="L25" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M25" s="24" t="s">
-        <v>30</v>
+      <c r="I25" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="K25" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="117.75" customHeight="1">
+    <row r="26" spans="1:11" ht="117.75" customHeight="1">
       <c r="A26" s="24">
         <v>19</v>
       </c>
-      <c r="B26" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="46">
+      <c r="B26" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="35">
         <v>1</v>
       </c>
-      <c r="E26" s="46">
+      <c r="E26" s="35">
         <v>3</v>
       </c>
-      <c r="F26" s="46">
+      <c r="F26" s="35">
         <v>3</v>
       </c>
       <c r="G26" s="25">
@@ -4642,123 +4491,105 @@
         <f>'Matriz de Riesgo'!$G$8:$G$26</f>
         <v>9</v>
       </c>
-      <c r="I26" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="K26" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L26" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M26" s="24" t="s">
-        <v>30</v>
+      <c r="I26" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="K26" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="59.25" customHeight="1">
+    <row r="27" spans="1:11" ht="59.25" customHeight="1">
       <c r="A27" s="24">
         <v>20</v>
       </c>
-      <c r="B27" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="46">
+      <c r="B27" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="35">
         <v>1</v>
       </c>
-      <c r="E27" s="46">
+      <c r="E27" s="35">
         <v>4</v>
       </c>
-      <c r="F27" s="46">
+      <c r="F27" s="35">
         <v>3</v>
       </c>
       <c r="G27" s="25">
-        <f>'Matriz de Riesgo'!$E$8:$E$39*'Matriz de Riesgo'!$F$8:$F$39</f>
+        <f>'Matriz de Riesgo'!$E$8:$E$37*'Matriz de Riesgo'!$F$8:$F$37</f>
         <v>12</v>
       </c>
       <c r="H27" s="25">
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>12</v>
       </c>
-      <c r="I27" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J27" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="K27" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="L27" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M27" s="24" t="s">
-        <v>30</v>
+      <c r="I27" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="K27" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="43.5" customHeight="1">
+    <row r="28" spans="1:11" ht="43.5" customHeight="1">
       <c r="A28" s="24">
         <v>21</v>
       </c>
-      <c r="B28" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="46">
+      <c r="B28" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="35">
         <v>1</v>
       </c>
-      <c r="E28" s="46">
+      <c r="E28" s="35">
         <v>3</v>
       </c>
-      <c r="F28" s="46">
+      <c r="F28" s="35">
         <v>4</v>
       </c>
       <c r="G28" s="25">
-        <f>'Matriz de Riesgo'!$E$8:$E$39*'Matriz de Riesgo'!$F$8:$F$39</f>
+        <f>'Matriz de Riesgo'!$E$8:$E$37*'Matriz de Riesgo'!$F$8:$F$37</f>
         <v>12</v>
       </c>
       <c r="H28" s="25">
-        <f>'Matriz de Riesgo'!$G$8:$G$39</f>
+        <f>'Matriz de Riesgo'!$G$8:$G$37</f>
         <v>12</v>
       </c>
-      <c r="I28" s="46"/>
-      <c r="J28" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="K28" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="L28" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M28" s="24" t="s">
-        <v>30</v>
+      <c r="I28" s="35"/>
+      <c r="J28" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="143.25" customHeight="1">
+    <row r="29" spans="1:11" ht="143.25" customHeight="1">
       <c r="A29" s="24">
         <v>22</v>
       </c>
-      <c r="B29" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="46">
+      <c r="B29" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="35">
         <v>1</v>
       </c>
-      <c r="E29" s="46">
+      <c r="E29" s="35">
         <v>3</v>
       </c>
-      <c r="F29" s="46">
+      <c r="F29" s="35">
         <v>5</v>
       </c>
       <c r="G29" s="25">
@@ -4769,39 +4600,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>15</v>
       </c>
-      <c r="I29" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="K29" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="L29" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="M29" s="24" t="s">
-        <v>30</v>
+      <c r="I29" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="K29" s="42" t="s">
+        <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="87.75" customHeight="1">
+    <row r="30" spans="1:11" ht="87.75" customHeight="1">
       <c r="A30" s="24">
         <v>23</v>
       </c>
-      <c r="B30" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="46">
+      <c r="B30" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="35">
         <v>1</v>
       </c>
-      <c r="E30" s="46">
+      <c r="E30" s="35">
         <v>3</v>
       </c>
-      <c r="F30" s="46">
+      <c r="F30" s="35">
         <v>3</v>
       </c>
       <c r="G30" s="25">
@@ -4812,39 +4637,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>9</v>
       </c>
-      <c r="I30" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J30" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="K30" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="L30" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M30" s="24" t="s">
-        <v>30</v>
+      <c r="I30" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="K30" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="56.25" customHeight="1">
+    <row r="31" spans="1:11" ht="56.25" customHeight="1">
       <c r="A31" s="24">
         <v>24</v>
       </c>
-      <c r="B31" s="50" t="s">
-        <v>136</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="46">
+      <c r="B31" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="35">
         <v>1</v>
       </c>
-      <c r="E31" s="46">
+      <c r="E31" s="35">
         <v>3</v>
       </c>
-      <c r="F31" s="46">
+      <c r="F31" s="35">
         <v>4</v>
       </c>
       <c r="G31" s="25">
@@ -4855,39 +4674,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>12</v>
       </c>
-      <c r="I31" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J31" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="K31" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="L31" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M31" s="24" t="s">
-        <v>30</v>
+      <c r="I31" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="K31" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="74.25" customHeight="1">
+    <row r="32" spans="1:11" ht="74.25" customHeight="1">
       <c r="A32" s="24">
         <v>25</v>
       </c>
-      <c r="B32" s="50" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="46">
+      <c r="B32" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="35">
         <v>1</v>
       </c>
-      <c r="E32" s="46">
+      <c r="E32" s="35">
         <v>3</v>
       </c>
-      <c r="F32" s="46">
+      <c r="F32" s="35">
         <v>4</v>
       </c>
       <c r="G32" s="25">
@@ -4898,39 +4711,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>12</v>
       </c>
-      <c r="I32" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J32" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="K32" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L32" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M32" s="24" t="s">
-        <v>30</v>
+      <c r="I32" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="K32" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="42.75" customHeight="1">
+    <row r="33" spans="1:11" ht="42.75" customHeight="1">
       <c r="A33" s="24">
         <v>26</v>
       </c>
-      <c r="B33" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="C33" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="46">
+      <c r="B33" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="35">
         <v>1</v>
       </c>
-      <c r="E33" s="46">
+      <c r="E33" s="35">
         <v>4</v>
       </c>
-      <c r="F33" s="46">
+      <c r="F33" s="35">
         <v>5</v>
       </c>
       <c r="G33" s="25">
@@ -4941,39 +4748,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>20</v>
       </c>
-      <c r="I33" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J33" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="K33" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L33" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="M33" s="24" t="s">
-        <v>30</v>
+      <c r="I33" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="K33" s="42" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="75" customHeight="1">
+    <row r="34" spans="1:11" ht="75" customHeight="1">
       <c r="A34" s="24">
         <v>27</v>
       </c>
-      <c r="B34" s="50" t="s">
-        <v>141</v>
-      </c>
-      <c r="C34" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="46">
+      <c r="B34" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="35">
         <v>1</v>
       </c>
-      <c r="E34" s="46">
+      <c r="E34" s="35">
         <v>3</v>
       </c>
-      <c r="F34" s="46">
+      <c r="F34" s="35">
         <v>4</v>
       </c>
       <c r="G34" s="25">
@@ -4984,39 +4785,33 @@
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>12</v>
       </c>
-      <c r="I34" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J34" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="K34" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L34" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M34" s="24" t="s">
-        <v>30</v>
+      <c r="I34" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="K34" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="58.5" customHeight="1">
+    <row r="35" spans="1:11" ht="58.5" customHeight="1">
       <c r="A35" s="24">
         <v>28</v>
       </c>
-      <c r="B35" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="46">
+      <c r="B35" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="35">
         <v>1</v>
       </c>
-      <c r="E35" s="46">
+      <c r="E35" s="35">
         <v>3</v>
       </c>
-      <c r="F35" s="46">
+      <c r="F35" s="35">
         <v>5</v>
       </c>
       <c r="G35" s="25">
@@ -5027,163 +4822,101 @@
         <f>'Matriz de Riesgo'!$G$8:$G$35</f>
         <v>15</v>
       </c>
-      <c r="I35" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J35" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="K35" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L35" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M35" s="24" t="s">
-        <v>30</v>
+      <c r="I35" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J35" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="K35" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="60" customHeight="1">
+    <row r="36" spans="1:11" ht="60" customHeight="1">
       <c r="A36" s="24">
         <v>29</v>
       </c>
-      <c r="B36" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" s="46" t="s">
+      <c r="B36" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="35">
+        <v>1</v>
+      </c>
+      <c r="E36" s="35">
+        <v>2</v>
+      </c>
+      <c r="F36" s="35">
+        <v>3</v>
+      </c>
+      <c r="G36" s="25">
+        <f>'Matriz de Riesgo'!$E$8:$E$37*'Matriz de Riesgo'!$F$8:$F$37</f>
+        <v>6</v>
+      </c>
+      <c r="H36" s="25">
+        <f>'Matriz de Riesgo'!$G$8:$G$37</f>
+        <v>6</v>
+      </c>
+      <c r="I36" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="46">
-        <v>1</v>
-      </c>
-      <c r="E36" s="46">
-        <v>2</v>
-      </c>
-      <c r="F36" s="46">
-        <v>3</v>
-      </c>
-      <c r="G36" s="25">
-        <f>'Matriz de Riesgo'!$E$8:$E$39*'Matriz de Riesgo'!$F$8:$F$39</f>
-        <v>6</v>
-      </c>
-      <c r="H36" s="25">
-        <f>'Matriz de Riesgo'!$G$8:$G$39</f>
-        <v>6</v>
-      </c>
-      <c r="I36" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J36" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="K36" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L36" s="53" t="s">
-        <v>76</v>
-      </c>
-      <c r="M36" s="24" t="s">
-        <v>30</v>
+      <c r="J36" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="K36" s="42" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="72.75" customHeight="1">
+    <row r="37" spans="1:11" ht="72.75" customHeight="1">
       <c r="A37" s="24">
         <v>30</v>
       </c>
-      <c r="B37" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="C37" s="46" t="s">
+      <c r="B37" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="35">
+        <v>1</v>
+      </c>
+      <c r="E37" s="35">
+        <v>2</v>
+      </c>
+      <c r="F37" s="35">
+        <v>4</v>
+      </c>
+      <c r="G37" s="25">
+        <f>'Matriz de Riesgo'!$E$8:$E$37*'Matriz de Riesgo'!$F$8:$F$37</f>
+        <v>8</v>
+      </c>
+      <c r="H37" s="25">
+        <f>'Matriz de Riesgo'!$G$8:$G$37</f>
+        <v>8</v>
+      </c>
+      <c r="I37" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="46">
-        <v>1</v>
-      </c>
-      <c r="E37" s="46">
-        <v>2</v>
-      </c>
-      <c r="F37" s="46">
-        <v>4</v>
-      </c>
-      <c r="G37" s="25">
-        <f>'Matriz de Riesgo'!$E$8:$E$39*'Matriz de Riesgo'!$F$8:$F$39</f>
-        <v>8</v>
-      </c>
-      <c r="H37" s="25">
-        <f>'Matriz de Riesgo'!$G$8:$G$39</f>
-        <v>8</v>
-      </c>
-      <c r="I37" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="J37" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="K37" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L37" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="M37" s="24" t="s">
-        <v>30</v>
+      <c r="J37" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="K37" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A38" s="24">
-        <v>31</v>
-      </c>
-      <c r="B38" s="42"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="28">
-        <f>'Matriz de Riesgo'!$E$8:$E$39*'Matriz de Riesgo'!$F$8:$F$39</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="28">
-        <f>'Matriz de Riesgo'!$G$8:$G$39</f>
-        <v>0</v>
-      </c>
-      <c r="I38" s="29"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-    </row>
-    <row r="39" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A39" s="24">
-        <v>32</v>
-      </c>
-      <c r="B39" s="42"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="28">
-        <f>'Matriz de Riesgo'!$E$8:$E$39*'Matriz de Riesgo'!$F$8:$F$39</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="28">
-        <f>'Matriz de Riesgo'!$G$8:$G$39</f>
-        <v>0</v>
-      </c>
-      <c r="I39" s="29"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
-    </row>
-    <row r="40" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:13" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -6134,22 +5867,20 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M6"/>
+    <mergeCell ref="A1:K6"/>
   </mergeCells>
-  <conditionalFormatting sqref="H8:H39">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="between">
+  <conditionalFormatting sqref="H8:H37">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>20</formula>
       <formula>25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>11</formula>
       <formula>19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>
@@ -6167,13 +5898,13 @@
           <x14:formula1>
             <xm:f>Tabla!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I8:I39</xm:sqref>
+          <xm:sqref>I8:I37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Tabla!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C8:C39</xm:sqref>
+          <xm:sqref>C8:C37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6211,174 +5942,174 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
       </c>
       <c r="J1" t="s">
         <v>19</v>
       </c>
       <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="34"/>
+      <c r="O1" s="47"/>
     </row>
     <row r="2" spans="1:15" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K2">
         <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K3">
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K4">
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
         <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" t="s">
-        <v>60</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K5">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="14.25" customHeight="1">
       <c r="F6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="14.25" customHeight="1"/>
@@ -6390,18 +6121,18 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" t="s">
         <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="14.25" customHeight="1">
@@ -6412,23 +6143,23 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:15" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="14.25" customHeight="1"/>

</xml_diff>